<commit_message>
likes db 오류 수정
</commit_message>
<xml_diff>
--- a/finalp/src/main/webapp/resources/db/LIKES.xlsx
+++ b/finalp/src/main/webapp/resources/db/LIKES.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FinalProjectWorkspace\finalp\src\main\webapp\resources\db\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="11835" windowHeight="4680"/>
+    <workbookView xWindow="240" yWindow="72" windowWidth="11832" windowHeight="4680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>PROJECT_ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -46,10 +51,6 @@
   </si>
   <si>
     <t>201803102301443</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>152140018016610</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -68,7 +69,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -125,6 +126,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -172,7 +176,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -207,7 +211,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -416,19 +420,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="17.25" customWidth="1"/>
-    <col min="2" max="2" width="12.125" customWidth="1"/>
+    <col min="1" max="1" width="17.19921875" customWidth="1"/>
+    <col min="2" max="2" width="12.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -436,7 +440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -444,7 +448,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -452,7 +456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -460,7 +464,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -468,7 +472,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -476,7 +480,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -484,7 +488,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -492,19 +496,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
         <v>2</v>
       </c>
     </row>
@@ -521,7 +517,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -534,7 +530,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>